<commit_message>
Add Graph for Output Voltage/Period Time
</commit_message>
<xml_diff>
--- a/measurements/converter_behaviour.xlsx
+++ b/measurements/converter_behaviour.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\benedikt.schmidt\Entwicklung\dcconverter\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1A3023-4883-47B3-AB6A-D848BD502561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D94047-DC03-49A8-B7CD-6647B9595C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82C672EE-2926-4EE4-9CCD-B56BCC1164F7}"/>
   </bookViews>
@@ -108,6 +108,1054 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Output Voltage [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>107.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.66</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F2F1-427D-99E0-D089D57ED069}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1031509376"/>
+        <c:axId val="1373184080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1031509376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Period</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" baseline="0"/>
+                  <a:t> Time [us]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1373184080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1373184080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Output Voltage [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1031509376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF854E57-8AAE-45B4-BBA9-FE841E855F0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,7 +1480,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,8 +1757,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>